<commit_message>
Add Xforce Exchange API request functionality for saving scores to spreadsheet
</commit_message>
<xml_diff>
--- a/ip_list.xlsx
+++ b/ip_list.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="14760"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="14760" windowWidth="28695"/>
   </bookViews>
   <sheets>
-    <sheet name="ReferenceData_Test_ThreatConnec" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ReferenceData_Test_ThreatConnec" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames/>
+  <calcPr calcId="144525" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="118">
   <si>
     <t>IP</t>
   </si>
@@ -374,180 +374,262 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  <numFmts count="3">
+    <numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" numFmtId="164"/>
+    <numFmt formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ " numFmtId="165"/>
+    <numFmt formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ " numFmtId="166"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <b val="1"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <color theme="0"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <charset val="134"/>
+      <color theme="3"/>
+      <sz val="18"/>
+      <scheme val="major"/>
+    </font>
+    <font>
       <name val="Calibri"/>
       <charset val="134"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF0000FF"/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <b val="1"/>
+      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <charset val="134"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="13"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <b val="1"/>
+      <color theme="0"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="15"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color rgb="FF9C0006"/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -559,169 +641,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,65 +724,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -819,6 +752,41 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -833,6 +801,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -841,135 +824,139 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="26" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="31" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="16" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="28" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="5" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="24" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="22" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="17" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="29" fontId="3" numFmtId="0"/>
+    <xf borderId="8" fillId="0" fontId="14" numFmtId="0"/>
+    <xf borderId="0" fillId="19" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="18" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="13" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="32" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="30" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="6" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="11" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="14" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="25" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="10" fontId="11" numFmtId="0"/>
+    <xf borderId="0" fillId="8" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="23" fontId="18" numFmtId="0"/>
+    <xf borderId="0" fillId="9" fontId="0" numFmtId="0"/>
+    <xf borderId="4" fillId="0" fontId="9" numFmtId="0"/>
+    <xf borderId="3" fillId="3" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="7" fontId="0" numFmtId="0"/>
+    <xf borderId="6" fillId="12" fontId="0" numFmtId="0"/>
+    <xf borderId="1" fillId="21" fontId="17" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0"/>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="20" fontId="15" numFmtId="0"/>
+    <xf borderId="2" fillId="0" fontId="6" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf borderId="9" fillId="0" fontId="16" numFmtId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="165">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="5" fillId="0" fontId="10" numFmtId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="166">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="7" fillId="15" fontId="12" numFmtId="0"/>
+    <xf borderId="0" fillId="27" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="1"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="2"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="3"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="4"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="5"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="6"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="7"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="8"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="9"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="10"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="11"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="12"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="13"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="14"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="16"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="17"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="18"/>
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="19"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="20"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="21"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="22"/>
+    <cellStyle builtinId="27" name="Bad" xfId="23"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="24"/>
+    <cellStyle builtinId="25" name="Total" xfId="25"/>
+    <cellStyle builtinId="21" name="Output" xfId="26"/>
+    <cellStyle builtinId="4" name="Currency" xfId="27"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="28"/>
+    <cellStyle builtinId="10" name="Note" xfId="29"/>
+    <cellStyle builtinId="20" name="Input" xfId="30"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="31"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="32"/>
+    <cellStyle builtinId="26" name="Good" xfId="33"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="34"/>
+    <cellStyle builtinId="53" name="CExplanatory Text" xfId="35"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="36"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="37"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="38"/>
+    <cellStyle builtinId="15" name="Title" xfId="39"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="40"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="41"/>
+    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="42"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="43"/>
+    <cellStyle builtinId="3" name="Comma" xfId="44"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="45"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="46"/>
+    <cellStyle builtinId="5" name="Percent" xfId="47"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="48"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -1229,18 +1216,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.8533333333333" customWidth="1"/>
-    <col min="2" max="2" width="12.7133333333333" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="14.8533333333333"/>
+    <col customWidth="1" max="2" min="2" width="12.7133333333333"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1255,602 +1245,940 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>8</v>
+      <c r="B2" t="n">
+        <v>5.7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B3" t="n">
+        <v>4.3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>3</v>
+      <c r="B4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>4</v>
+      <c r="B5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="B9" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34" t="n">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B35" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="B36" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="B37" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="B38" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="B39" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="B40" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="B41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="B42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
+      <c r="B43" t="n">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
+      <c r="B44" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
+      <c r="B45" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
+      <c r="B46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
+      <c r="B47" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="49" spans="1:1">
+      <c r="B48" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="B49" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="B50" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="B51" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="53" spans="1:1">
+      <c r="B52" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="54" spans="1:1">
+      <c r="B53" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="B54" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="B55" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="57" spans="1:1">
+      <c r="B56" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
+      <c r="B57" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
+      <c r="B58" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="60" spans="1:1">
+      <c r="B59" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
+      <c r="B60" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
+      <c r="B61" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="63" spans="1:1">
+      <c r="B62" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="64" spans="1:1">
+      <c r="B63" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
+      <c r="B64" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="66" spans="1:1">
+      <c r="B65" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="B66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="B67" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="69" spans="1:1">
+      <c r="B68" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="B69" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="71" spans="1:1">
+      <c r="B70" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
       <c r="A71" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="72" spans="1:1">
+      <c r="B71" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
       <c r="A72" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="B72" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="B73" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="75" spans="1:1">
+      <c r="B74" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="76" spans="1:1">
+      <c r="B75" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="77" spans="1:1">
+      <c r="B76" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="78" spans="1:1">
+      <c r="B77" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="79" spans="1:1">
+      <c r="B78" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
       <c r="A79" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="80" spans="1:1">
+      <c r="B79" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
       <c r="A80" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="81" spans="1:1">
+      <c r="B80" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
       <c r="A81" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="82" spans="1:1">
+      <c r="B81" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
       <c r="A82" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="83" spans="1:1">
+      <c r="B82" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
       <c r="A83" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="84" spans="1:1">
+      <c r="B83" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
       <c r="A84" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="85" spans="1:1">
+      <c r="B84" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
       <c r="A85" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="86" spans="1:1">
+      <c r="B85" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
       <c r="A86" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="87" spans="1:1">
+      <c r="B86" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
       <c r="A87" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="88" spans="1:1">
+      <c r="B87" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
       <c r="A88" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="89" spans="1:1">
+      <c r="B88" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
       <c r="A89" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="90" spans="1:1">
+      <c r="B89" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
       <c r="A90" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="91" spans="1:1">
+      <c r="B90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
       <c r="A91" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="92" spans="1:1">
+      <c r="B91" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
       <c r="A92" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="93" spans="1:1">
+      <c r="B92" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
       <c r="A93" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="94" spans="1:1">
+      <c r="B93" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
       <c r="A94" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="95" spans="1:1">
+      <c r="B94" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
       <c r="A95" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="96" spans="1:1">
+      <c r="B95" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
       <c r="A96" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="97" spans="1:1">
+      <c r="B96" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
       <c r="A97" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="98" spans="1:1">
+      <c r="B97" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
       <c r="A98" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="99" spans="1:1">
+      <c r="B98" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
       <c r="A99" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="100" spans="1:1">
+      <c r="B99" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
       <c r="A100" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="101" spans="1:1">
+      <c r="B100" t="n">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
       <c r="A101" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="102" spans="1:1">
+      <c r="B101" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
       <c r="A102" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="103" spans="1:1">
+      <c r="B102" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
       <c r="A103" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="104" spans="1:1">
+      <c r="B103" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
       <c r="A104" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="105" spans="1:1">
+      <c r="B104" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
       <c r="A105" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="106" spans="1:1">
+      <c r="B105" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
       <c r="A106" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="107" spans="1:1">
+      <c r="B106" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
       <c r="A107" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="108" spans="1:1">
+      <c r="B107" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
       <c r="A108" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="109" spans="1:1">
+      <c r="B108" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
       <c r="A109" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="110" spans="1:1">
+      <c r="B109" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
       <c r="A110" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="111" spans="1:1">
+      <c r="B110" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
       <c r="A111" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="112" spans="1:1">
+      <c r="B111" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
       <c r="A112" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="113" spans="1:1">
+      <c r="B112" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
       <c r="A113" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="114" spans="1:1">
+      <c r="B113" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
       <c r="A114" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="115" spans="1:1">
+      <c r="B114" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
       <c r="A115" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="116" spans="1:1">
+      <c r="B115" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
       <c r="A116" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="117" spans="1:1">
+      <c r="B116" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
       <c r="A117" t="s">
         <v>117</v>
       </c>
+      <c r="B117" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="1"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;1#&amp;"Arial"&amp;7 Sensitivity: Internal &amp; Restricted</oddFooter>
+    <oddHeader/>
+    <oddFooter>&amp;C&amp;"Arial"&amp;7 #Sensitivity: Internal &amp; Restricted</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add URL hyperlink to spreadsheets, rename API key file, include usage of key with Xforce Exchange.
</commit_message>
<xml_diff>
--- a/ip_list.xlsx
+++ b/ip_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="246">
   <si>
     <t>IP</t>
   </si>
@@ -25,382 +25,733 @@
     <t>Category</t>
   </si>
   <si>
+    <t>URL</t>
+  </si>
+  <si>
     <t>103.108.220.2</t>
   </si>
   <si>
     <t>Spam, Anonymisation Services</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/103.108.220.2</t>
+  </si>
+  <si>
     <t>103.224.212.222</t>
   </si>
   <si>
     <t>Anonymisation Services, Botnet Command and Control Server</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/103.224.212.222</t>
+  </si>
+  <si>
     <t>103.44.63.75</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/103.44.63.75</t>
+  </si>
+  <si>
     <t>104.131.161.182</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/104.131.161.182</t>
+  </si>
+  <si>
     <t>107.152.24.198</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/107.152.24.198</t>
+  </si>
+  <si>
     <t>107.152.25.198</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/107.152.25.198</t>
+  </si>
+  <si>
     <t>132.148.50.1</t>
   </si>
   <si>
     <t>Anonymisation Services</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/132.148.50.1</t>
+  </si>
+  <si>
     <t>141.8.224.93</t>
   </si>
   <si>
     <t>Anonymisation Services, Malware, Botnet Command and Control Server</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/141.8.224.93</t>
+  </si>
+  <si>
     <t>155.57.160.104</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/155.57.160.104</t>
+  </si>
+  <si>
     <t>162.125.7.1</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/162.125.7.1</t>
+  </si>
+  <si>
     <t>162.222.225.172</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/162.222.225.172</t>
+  </si>
+  <si>
     <t>172.17.30.28</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/172.17.30.28</t>
+  </si>
+  <si>
     <t>172.217.3.211</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/172.217.3.211</t>
+  </si>
+  <si>
     <t>172.22.114.66</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/172.22.114.66</t>
+  </si>
+  <si>
     <t>172.23.100.102</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/172.23.100.102</t>
+  </si>
+  <si>
     <t>172.23.165.31</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/172.23.165.31</t>
+  </si>
+  <si>
     <t>172.23.209.247</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/172.23.209.247</t>
+  </si>
+  <si>
     <t>172.23.210.14</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/172.23.210.14</t>
+  </si>
+  <si>
     <t>172.23.210.25</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/172.23.210.25</t>
+  </si>
+  <si>
     <t>172.23.48.53</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/172.23.48.53</t>
+  </si>
+  <si>
     <t>172.23.52.25</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/172.23.52.25</t>
+  </si>
+  <si>
     <t>172.23.56.70</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/172.23.56.70</t>
+  </si>
+  <si>
     <t>172.23.56.76</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/172.23.56.76</t>
+  </si>
+  <si>
     <t>172.23.58.20</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/172.23.58.20</t>
+  </si>
+  <si>
     <t>172.26.105.94</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/172.26.105.94</t>
+  </si>
+  <si>
     <t>172.26.40.21</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/172.26.40.21</t>
+  </si>
+  <si>
     <t>172.26.57.72</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/172.26.57.72</t>
+  </si>
+  <si>
     <t>173.201.93.128</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/173.201.93.128</t>
+  </si>
+  <si>
     <t>181.214.31.149</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/181.214.31.149</t>
+  </si>
+  <si>
     <t>184.168.185.1</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/184.168.185.1</t>
+  </si>
+  <si>
     <t>184.168.188.1</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/184.168.188.1</t>
+  </si>
+  <si>
     <t>184.168.190.1</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/184.168.190.1</t>
+  </si>
+  <si>
     <t>184.168.193.43</t>
   </si>
   <si>
     <t>Spam</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/184.168.193.43</t>
+  </si>
+  <si>
     <t>184.168.221.40</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/184.168.221.40</t>
+  </si>
+  <si>
     <t>184.168.221.45</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/184.168.221.45</t>
+  </si>
+  <si>
     <t>184.168.221.46</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/184.168.221.46</t>
+  </si>
+  <si>
     <t>184.168.221.47</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/184.168.221.47</t>
+  </si>
+  <si>
     <t>184.168.221.59</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/184.168.221.59</t>
+  </si>
+  <si>
     <t>184.168.221.68</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/184.168.221.68</t>
+  </si>
+  <si>
     <t>184.168.26.1</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/184.168.26.1</t>
+  </si>
+  <si>
     <t>184.168.46.18</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/184.168.46.18</t>
+  </si>
+  <si>
     <t>184.168.47.225</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/184.168.47.225</t>
+  </si>
+  <si>
     <t>185.151.28.157</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/185.151.28.157</t>
+  </si>
+  <si>
     <t>185.230.61.161</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/185.230.61.161</t>
+  </si>
+  <si>
     <t>185.230.61.164</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/185.230.61.164</t>
+  </si>
+  <si>
     <t>185.230.61.177</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/185.230.61.177</t>
+  </si>
+  <si>
     <t>185.53.178.9</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/185.53.178.9</t>
+  </si>
+  <si>
     <t>185.53.179.29</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/185.53.179.29</t>
+  </si>
+  <si>
     <t>185.53.179.8</t>
   </si>
   <si>
     <t>Anonymisation Services, Malware</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/185.53.179.8</t>
+  </si>
+  <si>
     <t>187.45.193.168</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/187.45.193.168</t>
+  </si>
+  <si>
     <t>192.124.249.152</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/192.124.249.152</t>
+  </si>
+  <si>
     <t>192.35.177.64</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/192.35.177.64</t>
+  </si>
+  <si>
     <t>194.187.98.166</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/194.187.98.166</t>
+  </si>
+  <si>
     <t>194.187.98.167</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/194.187.98.167</t>
+  </si>
+  <si>
     <t>194.187.98.168</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/194.187.98.168</t>
+  </si>
+  <si>
     <t>194.187.98.169</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/194.187.98.169</t>
+  </si>
+  <si>
     <t>194.187.98.221</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/194.187.98.221</t>
+  </si>
+  <si>
     <t>195.208.1.102</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/195.208.1.102</t>
+  </si>
+  <si>
     <t>195.208.1.103</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/195.208.1.103</t>
+  </si>
+  <si>
     <t>198.185.159.144</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/198.185.159.144</t>
+  </si>
+  <si>
     <t>198.46.81.186</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/198.46.81.186</t>
+  </si>
+  <si>
     <t>198.49.23.144</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/198.49.23.144</t>
+  </si>
+  <si>
     <t>198.54.115.179</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/198.54.115.179</t>
+  </si>
+  <si>
     <t>198.54.117.200</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/198.54.117.200</t>
+  </si>
+  <si>
     <t>199.188.200.148</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/199.188.200.148</t>
+  </si>
+  <si>
     <t>2.16.106.89</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/2.16.106.89</t>
+  </si>
+  <si>
     <t>203.170.87.225</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/203.170.87.225</t>
+  </si>
+  <si>
     <t>205.178.189.131</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/205.178.189.131</t>
+  </si>
+  <si>
     <t>208.91.197.132</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/208.91.197.132</t>
+  </si>
+  <si>
     <t>208.91.197.27</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/208.91.197.27</t>
+  </si>
+  <si>
     <t>208.91.197.91</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/208.91.197.91</t>
+  </si>
+  <si>
     <t>209.197.3.15</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/209.197.3.15</t>
+  </si>
+  <si>
     <t>209.99.40.227</t>
   </si>
   <si>
     <t>Botnet Command and Control Server</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/209.99.40.227</t>
+  </si>
+  <si>
     <t>213.186.33.5</t>
   </si>
   <si>
     <t>Anonymisation Services, Botnet Command and Control Server, Cryptocurrency Mining</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/213.186.33.5</t>
+  </si>
+  <si>
     <t>216.239.32.21</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/216.239.32.21</t>
+  </si>
+  <si>
     <t>216.40.47.17</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/216.40.47.17</t>
+  </si>
+  <si>
     <t>216.58.217.163</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/216.58.217.163</t>
+  </si>
+  <si>
     <t>217.70.184.38</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/217.70.184.38</t>
+  </si>
+  <si>
     <t>46.17.44.54</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/46.17.44.54</t>
+  </si>
+  <si>
     <t>46.30.213.223</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/46.30.213.223</t>
+  </si>
+  <si>
     <t>50.62.173.69</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/50.62.173.69</t>
+  </si>
+  <si>
     <t>50.62.26.129</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/50.62.26.129</t>
+  </si>
+  <si>
     <t>50.63.202.58</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/50.63.202.58</t>
+  </si>
+  <si>
     <t>50.63.202.74</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/50.63.202.74</t>
+  </si>
+  <si>
     <t>50.63.35.1</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/50.63.35.1</t>
+  </si>
+  <si>
     <t>50.63.37.1</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/50.63.37.1</t>
+  </si>
+  <si>
     <t>50.63.90.1</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/50.63.90.1</t>
+  </si>
+  <si>
     <t>50.63.95.1</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/50.63.95.1</t>
+  </si>
+  <si>
     <t>52.216.161.219</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/52.216.161.219</t>
+  </si>
+  <si>
     <t>52.58.78.16</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/52.58.78.16</t>
+  </si>
+  <si>
     <t>64.98.145.30</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/64.98.145.30</t>
+  </si>
+  <si>
     <t>67.214.175.69</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/67.214.175.69</t>
+  </si>
+  <si>
     <t>68.66.216.12</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/68.66.216.12</t>
+  </si>
+  <si>
     <t>69.89.31.156</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/69.89.31.156</t>
+  </si>
+  <si>
     <t>72.21.81.240</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/72.21.81.240</t>
+  </si>
+  <si>
     <t>72.52.4.90</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/72.52.4.90</t>
+  </si>
+  <si>
     <t>74.208.236.200</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/74.208.236.200</t>
+  </si>
+  <si>
     <t>78.47.139.102</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/78.47.139.102</t>
+  </si>
+  <si>
     <t>80.78.250.175</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/80.78.250.175</t>
+  </si>
+  <si>
     <t>81.169.145.158</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/81.169.145.158</t>
+  </si>
+  <si>
     <t>81.169.145.163</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/81.169.145.163</t>
+  </si>
+  <si>
     <t>81.169.145.171</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/81.169.145.171</t>
+  </si>
+  <si>
     <t>81.169.145.72</t>
   </si>
   <si>
     <t>Malware, Botnet Command and Control Server, Cryptocurrency Mining</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/81.169.145.72</t>
+  </si>
+  <si>
     <t>81.169.145.74</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/81.169.145.74</t>
+  </si>
+  <si>
     <t>81.169.145.78</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/81.169.145.78</t>
+  </si>
+  <si>
     <t>81.169.145.88</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/81.169.145.88</t>
+  </si>
+  <si>
     <t>81.169.145.92</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/81.169.145.92</t>
+  </si>
+  <si>
     <t>81.169.145.93</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/81.169.145.93</t>
+  </si>
+  <si>
     <t>87.240.129.133</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/87.240.129.133</t>
+  </si>
+  <si>
     <t>87.240.129.71</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/87.240.129.71</t>
+  </si>
+  <si>
     <t>87.240.129.72</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/87.240.129.72</t>
+  </si>
+  <si>
     <t>87.240.182.224</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/87.240.182.224</t>
+  </si>
+  <si>
     <t>90.156.201.38</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/90.156.201.38</t>
+  </si>
+  <si>
     <t>93.184.220.23</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/93.184.220.23</t>
+  </si>
+  <si>
     <t>94.73.146.147</t>
   </si>
   <si>
     <t>Spam, Scanning IPs</t>
   </si>
   <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/94.73.146.147</t>
+  </si>
+  <si>
     <t>94.73.149.51</t>
+  </si>
+  <si>
+    <t>https://exchange.xforce.ibmcloud.com/ip/94.73.149.51</t>
   </si>
 </sst>
 </file>
@@ -431,7 +782,7 @@
     <font>
       <name val="Calibri"/>
       <charset val="134"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -452,31 +803,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri Light"/>
-      <charset val="134"/>
-      <color theme="3"/>
-      <sz val="18"/>
-      <scheme val="major"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <name val="Calibri"/>
       <charset val="134"/>
       <color rgb="FFFF0000"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <color theme="0"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -491,24 +828,9 @@
     <font>
       <name val="Calibri"/>
       <charset val="134"/>
-      <color rgb="FF3F3F76"/>
+      <b val="1"/>
+      <color rgb="FF3F3F3F"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <i val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF800080"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -529,6 +851,28 @@
     <font>
       <name val="Calibri"/>
       <charset val="134"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri Light"/>
+      <charset val="134"/>
+      <color theme="3"/>
+      <sz val="18"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <color rgb="FF006100"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -536,15 +880,22 @@
     <font>
       <name val="Calibri"/>
       <charset val="134"/>
-      <b val="1"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
       <name val="Calibri"/>
       <charset val="134"/>
-      <color rgb="FF9C6500"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -566,7 +917,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,19 +1067,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -602,79 +1085,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -686,67 +1097,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -757,15 +1108,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -794,30 +1136,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.399975585192419"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -832,13 +1150,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -860,6 +1182,35 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.399975585192419"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thick">
         <color theme="4"/>
@@ -869,62 +1220,62 @@
   </borders>
   <cellStyleXfs count="49">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="20" fontId="7" numFmtId="0"/>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="32" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="22" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="27" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="28" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="29" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="15" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="30" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="25" fontId="2" numFmtId="0"/>
+    <xf borderId="8" fillId="0" fontId="17" numFmtId="0"/>
+    <xf borderId="0" fillId="21" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="20" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="12" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="17" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="26" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="19" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="11" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="31" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="6" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="32" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="30" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="27" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="7" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="29" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="14" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="25" fontId="7" numFmtId="0"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="24" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="26" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="23" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="28" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="3" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="22" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="18" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="21" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="19" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="17" fontId="17" numFmtId="0"/>
-    <xf borderId="0" fillId="16" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="13" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="12" fontId="0" numFmtId="0"/>
-    <xf borderId="7" fillId="0" fontId="13" numFmtId="0"/>
-    <xf borderId="8" fillId="8" fontId="16" numFmtId="0"/>
+    <xf borderId="0" fillId="24" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="14" fontId="12" numFmtId="0"/>
+    <xf borderId="0" fillId="6" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="13" fontId="10" numFmtId="0"/>
+    <xf borderId="0" fillId="23" fontId="0" numFmtId="0"/>
+    <xf borderId="6" fillId="0" fontId="9" numFmtId="0"/>
+    <xf borderId="5" fillId="8" fontId="8" numFmtId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="0" fillId="10" fontId="0" numFmtId="0"/>
-    <xf borderId="4" fillId="4" fontId="0" numFmtId="0"/>
-    <xf borderId="6" fillId="9" fontId="10" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0"/>
-    <xf borderId="6" fillId="8" fontId="9" numFmtId="0"/>
-    <xf borderId="0" fillId="15" fontId="15" numFmtId="0"/>
-    <xf borderId="5" fillId="0" fontId="8" numFmtId="0"/>
+    <xf borderId="4" fillId="9" fontId="0" numFmtId="0"/>
+    <xf borderId="3" fillId="18" fontId="15" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0"/>
+    <xf borderId="3" fillId="8" fontId="7" numFmtId="0"/>
+    <xf borderId="0" fillId="16" fontId="14" numFmtId="0"/>
+    <xf borderId="7" fillId="0" fontId="16" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0"/>
     <xf borderId="9" fillId="0" fontId="18" numFmtId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="165">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf borderId="0" fillId="7" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="12" numFmtId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0"/>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="166">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="11" fontId="7" numFmtId="0"/>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1254,20 +1605,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C117"/>
+  <dimension ref="A1:D117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="14.8533333333333"/>
     <col customWidth="1" max="2" min="2" width="12.7133333333333"/>
-    <col customWidth="1" max="3" min="3" width="42.1"/>
+    <col customWidth="1" max="3" min="3" width="76"/>
+    <col customWidth="1" max="4" min="4" width="50.6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1277,1168 +1629,1637 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="n">
         <v>4.3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" t="n">
         <v>4.3</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
       <c r="C4" t="s"/>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
       </c>
       <c r="C5" t="s"/>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B6" t="n">
         <v>1</v>
       </c>
       <c r="C6" t="s"/>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
       <c r="C7" t="s"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B8" t="n">
         <v>4.3</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B9" t="n">
         <v>4.3</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B10" t="n">
         <v>1</v>
       </c>
       <c r="C10" t="s"/>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
       <c r="C11" t="s"/>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="s"/>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="s"/>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s"/>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s"/>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s"/>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s"/>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s"/>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s"/>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s"/>
+      <c r="D20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s"/>
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s"/>
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s"/>
+      <c r="D23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s"/>
+      <c r="D24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s"/>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s"/>
+      <c r="D26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s"/>
+      <c r="D27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s"/>
+      <c r="D28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="C29" t="s">
         <v>19</v>
       </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" t="n">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="B30" t="n">
         <v>1</v>
       </c>
       <c r="C30" t="s"/>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="B31" t="n">
         <v>4.3</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="B32" t="n">
         <v>1</v>
       </c>
       <c r="C32" t="s"/>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="B33" t="n">
         <v>4.3</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="B34" t="n">
         <v>2.9</v>
       </c>
       <c r="C34" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>73</v>
+      </c>
+      <c r="D34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="B35" t="n">
         <v>4.3</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="B36" t="n">
         <v>4.3</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="D36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="B37" t="n">
         <v>4.3</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="B38" t="n">
         <v>4.3</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>22</v>
+      </c>
+      <c r="D38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="B39" t="n">
         <v>4.3</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="D39" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="B40" t="n">
         <v>4.3</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="D40" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="B41" t="n">
         <v>1</v>
       </c>
       <c r="C41" t="s"/>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="D41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="B42" t="n">
         <v>1</v>
       </c>
       <c r="C42" t="s"/>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="D42" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="B43" t="n">
         <v>2.9</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="D43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="B44" t="n">
         <v>4.3</v>
       </c>
       <c r="C44" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D44" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="B45" t="n">
         <v>1</v>
       </c>
       <c r="C45" t="s"/>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="D45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="B46" t="n">
         <v>1</v>
       </c>
       <c r="C46" t="s"/>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="D46" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="B47" t="n">
         <v>1</v>
       </c>
       <c r="C47" t="s"/>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>101</v>
       </c>
       <c r="B48" t="n">
         <v>4.3</v>
       </c>
       <c r="C48" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>22</v>
+      </c>
+      <c r="D48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="B49" t="n">
         <v>4.3</v>
       </c>
       <c r="C49" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>22</v>
+      </c>
+      <c r="D49" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="B50" t="n">
         <v>4.3</v>
       </c>
       <c r="C50" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>106</v>
+      </c>
+      <c r="D50" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="B51" t="n">
         <v>4.3</v>
       </c>
       <c r="C51" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D51" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="B52" t="n">
         <v>4.3</v>
       </c>
       <c r="C52" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D52" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="B53" t="n">
         <v>1</v>
       </c>
       <c r="C53" t="s"/>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="D53" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>61</v>
+        <v>114</v>
       </c>
       <c r="B54" t="n">
         <v>1</v>
       </c>
       <c r="C54" t="s"/>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="D54" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>116</v>
       </c>
       <c r="B55" t="n">
         <v>1</v>
       </c>
       <c r="C55" t="s"/>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="D55" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="B56" t="n">
         <v>1</v>
       </c>
       <c r="C56" t="s"/>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="D56" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="B57" t="n">
         <v>1</v>
       </c>
       <c r="C57" t="s"/>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="D57" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>122</v>
       </c>
       <c r="B58" t="n">
         <v>1</v>
       </c>
       <c r="C58" t="s"/>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="D58" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
       <c r="B59" t="n">
         <v>4.3</v>
       </c>
       <c r="C59" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D59" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="B60" t="n">
         <v>4.3</v>
       </c>
       <c r="C60" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D60" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>68</v>
+        <v>128</v>
       </c>
       <c r="B61" t="n">
         <v>4.3</v>
       </c>
       <c r="C61" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
+        <v>22</v>
+      </c>
+      <c r="D61" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
       <c r="B62" t="n">
         <v>1</v>
       </c>
       <c r="C62" t="s"/>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="D62" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="B63" t="n">
         <v>4.3</v>
       </c>
       <c r="C63" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
+        <v>22</v>
+      </c>
+      <c r="D63" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>71</v>
+        <v>134</v>
       </c>
       <c r="B64" t="n">
         <v>1</v>
       </c>
       <c r="C64" t="s"/>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="D64" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="B65" t="n">
         <v>4.3</v>
       </c>
       <c r="C65" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
+        <v>22</v>
+      </c>
+      <c r="D65" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>73</v>
+        <v>138</v>
       </c>
       <c r="B66" t="n">
         <v>1</v>
       </c>
       <c r="C66" t="s"/>
-    </row>
-    <row r="67" spans="1:3">
+      <c r="D66" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>74</v>
+        <v>140</v>
       </c>
       <c r="B67" t="n">
         <v>1</v>
       </c>
       <c r="C67" t="s"/>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="D67" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>75</v>
+        <v>142</v>
       </c>
       <c r="B68" t="n">
         <v>1</v>
       </c>
       <c r="C68" t="s"/>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="D68" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>76</v>
+        <v>144</v>
       </c>
       <c r="B69" t="n">
         <v>4.3</v>
       </c>
       <c r="C69" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
+        <v>22</v>
+      </c>
+      <c r="D69" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>77</v>
+        <v>146</v>
       </c>
       <c r="B70" t="n">
         <v>4.3</v>
       </c>
       <c r="C70" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="D70" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>78</v>
+        <v>148</v>
       </c>
       <c r="B71" t="n">
         <v>4.3</v>
       </c>
       <c r="C71" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="D71" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>79</v>
+        <v>150</v>
       </c>
       <c r="B72" t="n">
         <v>4.3</v>
       </c>
       <c r="C72" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="D72" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>80</v>
+        <v>152</v>
       </c>
       <c r="B73" t="n">
         <v>1</v>
       </c>
       <c r="C73" t="s"/>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="D73" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>81</v>
+        <v>154</v>
       </c>
       <c r="B74" t="n">
         <v>4.3</v>
       </c>
       <c r="C74" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
+        <v>155</v>
+      </c>
+      <c r="D74" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>83</v>
+        <v>157</v>
       </c>
       <c r="B75" t="n">
         <v>4.3</v>
       </c>
       <c r="C75" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
+        <v>158</v>
+      </c>
+      <c r="D75" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="B76" t="n">
         <v>4.3</v>
       </c>
       <c r="C76" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
+        <v>106</v>
+      </c>
+      <c r="D76" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="B77" t="n">
         <v>4.3</v>
       </c>
       <c r="C77" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
+        <v>22</v>
+      </c>
+      <c r="D77" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="B78" t="n">
         <v>1</v>
       </c>
       <c r="C78" t="s"/>
-    </row>
-    <row r="79" spans="1:3">
+      <c r="D78" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>88</v>
+        <v>166</v>
       </c>
       <c r="B79" t="n">
         <v>4.3</v>
       </c>
       <c r="C79" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
+        <v>155</v>
+      </c>
+      <c r="D79" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>89</v>
+        <v>168</v>
       </c>
       <c r="B80" t="n">
         <v>1.4</v>
       </c>
       <c r="C80" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
+        <v>155</v>
+      </c>
+      <c r="D80" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="B81" t="n">
         <v>1</v>
       </c>
       <c r="C81" t="s"/>
-    </row>
-    <row r="82" spans="1:3">
+      <c r="D81" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>91</v>
+        <v>172</v>
       </c>
       <c r="B82" t="n">
         <v>4.3</v>
       </c>
       <c r="C82" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D82" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B83" t="n">
         <v>4.3</v>
       </c>
       <c r="C83" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D83" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>93</v>
+        <v>176</v>
       </c>
       <c r="B84" t="n">
         <v>4.3</v>
       </c>
       <c r="C84" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="D84" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>178</v>
       </c>
       <c r="B85" t="n">
         <v>4.3</v>
       </c>
       <c r="C85" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="D85" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="B86" t="n">
         <v>1</v>
       </c>
       <c r="C86" t="s"/>
-    </row>
-    <row r="87" spans="1:3">
+      <c r="D86" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>96</v>
+        <v>182</v>
       </c>
       <c r="B87" t="n">
         <v>1</v>
       </c>
       <c r="C87" t="s"/>
-    </row>
-    <row r="88" spans="1:3">
+      <c r="D87" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>97</v>
+        <v>184</v>
       </c>
       <c r="B88" t="n">
         <v>1</v>
       </c>
       <c r="C88" t="s"/>
-    </row>
-    <row r="89" spans="1:3">
+      <c r="D88" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>186</v>
       </c>
       <c r="B89" t="n">
         <v>4.3</v>
       </c>
       <c r="C89" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D89" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>99</v>
+        <v>188</v>
       </c>
       <c r="B90" t="n">
         <v>1</v>
       </c>
       <c r="C90" t="s"/>
-    </row>
-    <row r="91" spans="1:3">
+      <c r="D90" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>100</v>
+        <v>190</v>
       </c>
       <c r="B91" t="n">
         <v>4.3</v>
       </c>
       <c r="C91" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="D91" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>101</v>
+        <v>192</v>
       </c>
       <c r="B92" t="n">
         <v>4.3</v>
       </c>
       <c r="C92" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D92" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>102</v>
+        <v>194</v>
       </c>
       <c r="B93" t="n">
         <v>5.7</v>
       </c>
       <c r="C93" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
+        <v>155</v>
+      </c>
+      <c r="D93" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>103</v>
+        <v>196</v>
       </c>
       <c r="B94" t="n">
         <v>4.3</v>
       </c>
       <c r="C94" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D94" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>104</v>
+        <v>198</v>
       </c>
       <c r="B95" t="n">
         <v>1</v>
       </c>
       <c r="C95" t="s"/>
-    </row>
-    <row r="96" spans="1:3">
+      <c r="D95" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>105</v>
+        <v>200</v>
       </c>
       <c r="B96" t="n">
         <v>1</v>
       </c>
       <c r="C96" t="s"/>
-    </row>
-    <row r="97" spans="1:3">
+      <c r="D96" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>106</v>
+        <v>202</v>
       </c>
       <c r="B97" t="n">
         <v>4.3</v>
       </c>
       <c r="C97" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
+        <v>22</v>
+      </c>
+      <c r="D97" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>107</v>
+        <v>204</v>
       </c>
       <c r="B98" t="n">
         <v>1</v>
       </c>
       <c r="C98" t="s"/>
-    </row>
-    <row r="99" spans="1:3">
+      <c r="D98" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>108</v>
+        <v>206</v>
       </c>
       <c r="B99" t="n">
         <v>1</v>
       </c>
       <c r="C99" t="s"/>
-    </row>
-    <row r="100" spans="1:3">
+      <c r="D99" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>109</v>
+        <v>208</v>
       </c>
       <c r="B100" t="n">
         <v>2.9</v>
       </c>
       <c r="C100" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
+        <v>73</v>
+      </c>
+      <c r="D100" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>110</v>
+        <v>210</v>
       </c>
       <c r="B101" t="n">
         <v>4.3</v>
       </c>
       <c r="C101" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
+        <v>106</v>
+      </c>
+      <c r="D101" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>111</v>
+        <v>212</v>
       </c>
       <c r="B102" t="n">
         <v>4.3</v>
       </c>
       <c r="C102" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
+        <v>106</v>
+      </c>
+      <c r="D102" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>112</v>
+        <v>214</v>
       </c>
       <c r="B103" t="n">
         <v>1</v>
       </c>
       <c r="C103" t="s"/>
-    </row>
-    <row r="104" spans="1:3">
+      <c r="D103" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>113</v>
+        <v>216</v>
       </c>
       <c r="B104" t="n">
         <v>4.3</v>
       </c>
       <c r="C104" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
+        <v>217</v>
+      </c>
+      <c r="D104" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>115</v>
+        <v>219</v>
       </c>
       <c r="B105" t="n">
         <v>4.3</v>
       </c>
       <c r="C105" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
+        <v>106</v>
+      </c>
+      <c r="D105" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>116</v>
+        <v>221</v>
       </c>
       <c r="B106" t="n">
         <v>4.3</v>
       </c>
       <c r="C106" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
+        <v>106</v>
+      </c>
+      <c r="D106" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>117</v>
+        <v>223</v>
       </c>
       <c r="B107" t="n">
         <v>4.3</v>
       </c>
       <c r="C107" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
+        <v>22</v>
+      </c>
+      <c r="D107" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>118</v>
+        <v>225</v>
       </c>
       <c r="B108" t="n">
         <v>4.3</v>
       </c>
       <c r="C108" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
+        <v>106</v>
+      </c>
+      <c r="D108" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>119</v>
+        <v>227</v>
       </c>
       <c r="B109" t="n">
         <v>4.3</v>
       </c>
       <c r="C109" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D109" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>120</v>
+        <v>229</v>
       </c>
       <c r="B110" t="n">
         <v>1</v>
       </c>
       <c r="C110" t="s"/>
-    </row>
-    <row r="111" spans="1:3">
+      <c r="D110" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>121</v>
+        <v>231</v>
       </c>
       <c r="B111" t="n">
         <v>1</v>
       </c>
       <c r="C111" t="s"/>
-    </row>
-    <row r="112" spans="1:3">
+      <c r="D111" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>122</v>
+        <v>233</v>
       </c>
       <c r="B112" t="n">
         <v>1</v>
       </c>
       <c r="C112" t="s"/>
-    </row>
-    <row r="113" spans="1:3">
+      <c r="D112" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>123</v>
+        <v>235</v>
       </c>
       <c r="B113" t="n">
         <v>1</v>
       </c>
       <c r="C113" t="s"/>
-    </row>
-    <row r="114" spans="1:3">
+      <c r="D113" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>124</v>
+        <v>237</v>
       </c>
       <c r="B114" t="n">
         <v>4.3</v>
       </c>
       <c r="C114" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D114" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>125</v>
+        <v>239</v>
       </c>
       <c r="B115" t="n">
         <v>4.3</v>
       </c>
       <c r="C115" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D115" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>126</v>
+        <v>241</v>
       </c>
       <c r="B116" t="n">
         <v>4.3</v>
       </c>
       <c r="C116" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
+        <v>242</v>
+      </c>
+      <c r="D116" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>128</v>
+        <v>244</v>
       </c>
       <c r="B117" t="n">
         <v>1</v>
       </c>
       <c r="C117" t="s"/>
+      <c r="D117" t="s">
+        <v>245</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D4" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D5" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D6" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D7" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D8" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D9" r:id="rId8"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D10" r:id="rId9"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D11" r:id="rId10"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D12" r:id="rId11"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D13" r:id="rId12"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D14" r:id="rId13"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D15" r:id="rId14"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D16" r:id="rId15"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D17" r:id="rId16"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D18" r:id="rId17"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D19" r:id="rId18"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D20" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D21" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D22" r:id="rId21"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D23" r:id="rId22"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D24" r:id="rId23"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D25" r:id="rId24"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D26" r:id="rId25"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D27" r:id="rId26"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D28" r:id="rId27"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D29" r:id="rId28"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D30" r:id="rId29"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D31" r:id="rId30"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D32" r:id="rId31"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D33" r:id="rId32"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D34" r:id="rId33"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D35" r:id="rId34"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D36" r:id="rId35"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D37" r:id="rId36"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D38" r:id="rId37"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D39" r:id="rId38"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D40" r:id="rId39"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D41" r:id="rId40"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D42" r:id="rId41"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D43" r:id="rId42"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D44" r:id="rId43"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D45" r:id="rId44"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D46" r:id="rId45"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D47" r:id="rId46"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D48" r:id="rId47"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D49" r:id="rId48"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D50" r:id="rId49"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D51" r:id="rId50"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D52" r:id="rId51"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D53" r:id="rId52"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D54" r:id="rId53"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D55" r:id="rId54"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D56" r:id="rId55"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D57" r:id="rId56"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D58" r:id="rId57"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D59" r:id="rId58"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D60" r:id="rId59"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D61" r:id="rId60"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D62" r:id="rId61"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D63" r:id="rId62"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D64" r:id="rId63"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D65" r:id="rId64"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D66" r:id="rId65"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D67" r:id="rId66"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D68" r:id="rId67"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D69" r:id="rId68"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D70" r:id="rId69"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D71" r:id="rId70"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D72" r:id="rId71"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D73" r:id="rId72"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D74" r:id="rId73"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D75" r:id="rId74"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D76" r:id="rId75"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D77" r:id="rId76"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D78" r:id="rId77"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D79" r:id="rId78"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D80" r:id="rId79"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D81" r:id="rId80"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D82" r:id="rId81"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D83" r:id="rId82"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D84" r:id="rId83"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D85" r:id="rId84"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D86" r:id="rId85"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D87" r:id="rId86"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D88" r:id="rId87"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D89" r:id="rId88"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D90" r:id="rId89"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D91" r:id="rId90"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D92" r:id="rId91"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D93" r:id="rId92"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D94" r:id="rId93"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D95" r:id="rId94"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D96" r:id="rId95"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D97" r:id="rId96"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D98" r:id="rId97"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D99" r:id="rId98"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D100" r:id="rId99"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D101" r:id="rId100"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D102" r:id="rId101"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D103" r:id="rId102"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D104" r:id="rId103"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D105" r:id="rId104"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D106" r:id="rId105"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D107" r:id="rId106"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D108" r:id="rId107"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D109" r:id="rId108"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D110" r:id="rId109"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D111" r:id="rId110"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D112" r:id="rId111"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D113" r:id="rId112"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D114" r:id="rId113"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D115" r:id="rId114"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D116" r:id="rId115"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D117" r:id="rId116"/>
+  </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="1"/>
   <headerFooter>

</xml_diff>